<commit_message>
Fixed code to run despite issues occured
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis/output/tables/unbiassdness_e_m.xlsx
+++ b/gdp_revisions_analysis/output/tables/unbiassdness_e_m.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/Research Assistant/CIUP/GDP Revisions/GitHub/peru_gdp_revisions/gdp_revisions_analysis/output/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{93F9ABDE-F0F2-437C-8387-4F37526E42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4824ECA5-B68C-4ED6-8E9E-B13C45FF9698}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{93F9ABDE-F0F2-437C-8387-4F37526E42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2CCBB3A-307B-489E-AD3B-999172C77E11}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59A818B8-AC1C-48B4-9EC6-7BF703468C77}"/>
   </bookViews>
@@ -203,22 +203,7 @@
     <t>0.104**</t>
   </si>
   <si>
-    <t>N° de observaciones</t>
-  </si>
-  <si>
     <t>Media</t>
-  </si>
-  <si>
-    <t>Desviación Estándar</t>
-  </si>
-  <si>
-    <t>Percentil 1</t>
-  </si>
-  <si>
-    <t>Percentil 99</t>
-  </si>
-  <si>
-    <t>Horizonte (h)</t>
   </si>
   <si>
     <t>PBI</t>
@@ -246,6 +231,21 @@
   </si>
   <si>
     <t>Otros Servicios</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P99</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -9544,38 +9544,38 @@
   <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="1"/>
-    <col min="4" max="4" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -9583,7 +9583,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -10030,7 +10030,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -10477,7 +10477,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -10924,7 +10924,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -11371,7 +11371,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -11818,7 +11818,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -12150,7 +12150,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
@@ -12597,7 +12597,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
@@ -13044,7 +13044,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>

</xml_diff>

<commit_message>
Changed datasets loaded from SQL
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis/output/tables/unbiassdness_e_m.xlsx
+++ b/gdp_revisions_analysis/output/tables/unbiassdness_e_m.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/Research Assistant/CIUP/GDP Revisions/GitHub/peru_gdp_revisions/gdp_revisions_analysis/output/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{93F9ABDE-F0F2-437C-8387-4F37526E42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2CCBB3A-307B-489E-AD3B-999172C77E11}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{93F9ABDE-F0F2-437C-8387-4F37526E42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5929BAC3-36F1-4850-BB99-E69501CB7970}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59A818B8-AC1C-48B4-9EC6-7BF703468C77}"/>
   </bookViews>
@@ -36,75 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="69">
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>0.313***</t>
-  </si>
-  <si>
-    <t>0.255***</t>
-  </si>
-  <si>
-    <t>0.171***</t>
-  </si>
-  <si>
-    <t>0.110***</t>
-  </si>
-  <si>
-    <t>0.086***</t>
   </si>
   <si>
     <t>0.058**</t>
   </si>
   <si>
-    <t>0.791***</t>
-  </si>
-  <si>
-    <t>0.750***</t>
-  </si>
-  <si>
-    <t>0.598***</t>
-  </si>
-  <si>
-    <t>0.409***</t>
-  </si>
-  <si>
-    <t>0.304***</t>
-  </si>
-  <si>
-    <t>0.227***</t>
-  </si>
-  <si>
-    <t>0.163***</t>
-  </si>
-  <si>
     <t>0.134***</t>
-  </si>
-  <si>
-    <t>0.089***</t>
-  </si>
-  <si>
-    <t>0.055*</t>
-  </si>
-  <si>
-    <t>0.039*</t>
-  </si>
-  <si>
-    <t>1.569***</t>
-  </si>
-  <si>
-    <t>1.467***</t>
-  </si>
-  <si>
-    <t>1.256***</t>
-  </si>
-  <si>
-    <t>-0.352**</t>
-  </si>
-  <si>
-    <t>-0.251*</t>
   </si>
   <si>
     <t>0.438***</t>
@@ -246,6 +186,63 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>0.272***</t>
+  </si>
+  <si>
+    <t>0.204***</t>
+  </si>
+  <si>
+    <t>0.124***</t>
+  </si>
+  <si>
+    <t>0.068*</t>
+  </si>
+  <si>
+    <t>0.792***</t>
+  </si>
+  <si>
+    <t>0.745***</t>
+  </si>
+  <si>
+    <t>0.584***</t>
+  </si>
+  <si>
+    <t>0.401***</t>
+  </si>
+  <si>
+    <t>0.290***</t>
+  </si>
+  <si>
+    <t>0.208***</t>
+  </si>
+  <si>
+    <t>0.144***</t>
+  </si>
+  <si>
+    <t>0.113***</t>
+  </si>
+  <si>
+    <t>0.073**</t>
+  </si>
+  <si>
+    <t>0.053*</t>
+  </si>
+  <si>
+    <t>0.043*</t>
+  </si>
+  <si>
+    <t>1.326*</t>
+  </si>
+  <si>
+    <t>0.914*</t>
+  </si>
+  <si>
+    <t>-0.458**</t>
+  </si>
+  <si>
+    <t>-0.234*</t>
   </si>
 </sst>
 </file>
@@ -514,51 +511,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$3:$D$21</c:f>
+              <c:f>Hoja1!$F$3:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.80700000000000005</c:v>
+                  <c:v>0.96799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69899999999999995</c:v>
+                  <c:v>0.872</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66900000000000004</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58099999999999996</c:v>
+                  <c:v>0.73199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48699999999999999</c:v>
+                  <c:v>0.65600000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47099999999999997</c:v>
+                  <c:v>0.56499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43</c:v>
+                  <c:v>0.495</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.42099999999999999</c:v>
+                  <c:v>0.46100000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39100000000000001</c:v>
+                  <c:v>0.43099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34899999999999998</c:v>
+                  <c:v>0.38400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30299999999999999</c:v>
+                  <c:v>0.35599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.188</c:v>
+                  <c:v>0.23899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.121</c:v>
+                  <c:v>0.11700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26800000000000002</c:v>
+                  <c:v>0.26600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.252</c:v>
@@ -910,51 +907,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$23:$D$41</c:f>
+              <c:f>Hoja1!$F$23:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>1.7749999999999999</c:v>
+                  <c:v>1.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.506</c:v>
+                  <c:v>1.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.216</c:v>
+                  <c:v>1.278</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.117</c:v>
+                  <c:v>1.1759999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.036</c:v>
+                  <c:v>1.093</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98399999999999999</c:v>
+                  <c:v>1.042</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88700000000000001</c:v>
+                  <c:v>0.91200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.74199999999999999</c:v>
+                  <c:v>0.78300000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60499999999999998</c:v>
+                  <c:v>0.65100000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.55200000000000005</c:v>
+                  <c:v>0.58599999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.434</c:v>
+                  <c:v>0.46200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.318</c:v>
+                  <c:v>0.32100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.218</c:v>
+                  <c:v>0.21099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.313</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.38100000000000001</c:v>
@@ -1306,51 +1303,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$43:$D$61</c:f>
+              <c:f>Hoja1!$F$43:$F$61</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>8.2759999999999998</c:v>
+                  <c:v>15.125999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0370000000000008</c:v>
+                  <c:v>14.43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4060000000000006</c:v>
+                  <c:v>10.24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4039999999999999</c:v>
+                  <c:v>9.2550000000000008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8289999999999997</c:v>
+                  <c:v>7.9489999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.3179999999999996</c:v>
+                  <c:v>7.3220000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.1660000000000004</c:v>
+                  <c:v>7.6859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.2720000000000002</c:v>
+                  <c:v>6.84</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5270000000000001</c:v>
+                  <c:v>6.2130000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0359999999999996</c:v>
+                  <c:v>5.6440000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.496</c:v>
+                  <c:v>5.3079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.29</c:v>
+                  <c:v>4.3289999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.59</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.7850000000000001</c:v>
+                  <c:v>5.7380000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>6.1829999999999998</c:v>
@@ -8899,16 +8896,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8935,16 +8932,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8971,16 +8968,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9007,16 +9004,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9043,16 +9040,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9079,16 +9076,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:rowOff>186690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9115,16 +9112,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>678180</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>134</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9151,16 +9148,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>194310</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9187,16 +9184,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>157</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>739140</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>171</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9544,46 +9541,43 @@
   <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -9599,16 +9593,16 @@
         <v>372</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D3" s="5">
-        <v>0.80700000000000005</v>
+        <v>-3.3</v>
       </c>
       <c r="E3" s="5">
-        <v>-1.8</v>
+        <v>3.2</v>
       </c>
       <c r="F3" s="5">
-        <v>3.1</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>0</v>
@@ -9619,19 +9613,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2">
-        <v>0.69899999999999995</v>
+        <v>-3.4</v>
       </c>
       <c r="E4" s="2">
-        <v>-1.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F4" s="2">
-        <v>2.2000000000000002</v>
+        <v>0.872</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>0</v>
@@ -9642,19 +9636,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2">
-        <v>0.66900000000000004</v>
+        <v>-3.4</v>
       </c>
       <c r="E5" s="2">
-        <v>-1.6</v>
+        <v>1.8</v>
       </c>
       <c r="F5" s="2">
-        <v>1.9</v>
+        <v>0.81</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>0</v>
@@ -9665,19 +9659,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2">
-        <v>0.58099999999999996</v>
+        <v>-3.1</v>
       </c>
       <c r="E6" s="2">
-        <v>-1.7</v>
+        <v>1.7</v>
       </c>
       <c r="F6" s="2">
-        <v>1.7</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>0</v>
@@ -9688,19 +9682,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>364</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>372</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>0.48699999999999999</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="E7" s="2">
-        <v>-1.4</v>
+        <v>1.7</v>
       </c>
       <c r="F7" s="2">
-        <v>1.7</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>0</v>
@@ -9711,19 +9705,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>361</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>371</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>0.47099999999999997</v>
+        <v>-2</v>
       </c>
       <c r="E8" s="2">
-        <v>-1.4</v>
+        <v>1.6</v>
       </c>
       <c r="F8" s="2">
-        <v>1.4</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>0</v>
@@ -9734,19 +9728,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="C9" s="2">
-        <v>0.03</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D9" s="2">
-        <v>0.43</v>
+        <v>-1.8</v>
       </c>
       <c r="E9" s="2">
-        <v>-1.4</v>
+        <v>1.3</v>
       </c>
       <c r="F9" s="2">
-        <v>1.2</v>
+        <v>0.495</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>0</v>
@@ -9757,19 +9751,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="C10" s="2">
-        <v>1.9E-2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>0.42099999999999999</v>
+        <v>-1.5</v>
       </c>
       <c r="E10" s="2">
-        <v>-1.4</v>
+        <v>1.2</v>
       </c>
       <c r="F10" s="2">
-        <v>1.2</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>0</v>
@@ -9780,19 +9774,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="C11" s="2">
-        <v>1.0999999999999999E-2</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="D11" s="2">
-        <v>0.39100000000000001</v>
+        <v>-1.5</v>
       </c>
       <c r="E11" s="2">
-        <v>-1.4</v>
+        <v>1.2</v>
       </c>
       <c r="F11" s="2">
-        <v>1.2</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>0</v>
@@ -9803,19 +9797,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="C12" s="2">
-        <v>1.2E-2</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="D12" s="2">
-        <v>0.34899999999999998</v>
+        <v>-1.4</v>
       </c>
       <c r="E12" s="2">
-        <v>-1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="F12" s="2">
-        <v>1.2</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>0</v>
@@ -9826,19 +9820,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="C13" s="2">
-        <v>8.0000000000000002E-3</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="D13" s="2">
-        <v>0.30299999999999999</v>
+        <v>-1.2</v>
       </c>
       <c r="E13" s="2">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="F13" s="2">
-        <v>0.8</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>0</v>
@@ -9849,19 +9843,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="C14" s="2">
-        <v>-2E-3</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="D14" s="2">
-        <v>0.188</v>
+        <v>-0.7</v>
       </c>
       <c r="E14" s="2">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="F14" s="2">
-        <v>0.6</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>0</v>
@@ -9872,19 +9866,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="C15" s="2">
-        <v>-8.0000000000000002E-3</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="D15" s="2">
-        <v>0.121</v>
+        <v>-0.5</v>
       </c>
       <c r="E15" s="2">
-        <v>-0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F15" s="2">
-        <v>0.4</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>0</v>
@@ -9895,19 +9889,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="2">
-        <v>-1.9E-2</v>
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="D16" s="2">
-        <v>0.26800000000000002</v>
+        <v>-1.2</v>
       </c>
       <c r="E16" s="2">
-        <v>-1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F16" s="2">
-        <v>0.6</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>0</v>
@@ -9924,13 +9918,13 @@
         <v>-0.02</v>
       </c>
       <c r="D17" s="2">
+        <v>-0.8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="F17" s="2">
         <v>0.252</v>
-      </c>
-      <c r="E17" s="2">
-        <v>-0.8</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.6</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>0</v>
@@ -9947,13 +9941,13 @@
         <v>-4.0000000000000001E-3</v>
       </c>
       <c r="D18" s="2">
+        <v>-0.7</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="F18" s="2">
         <v>0.193</v>
-      </c>
-      <c r="E18" s="2">
-        <v>-0.7</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.6</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>0</v>
@@ -9970,13 +9964,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D19" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="2">
         <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="E19" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.1</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>0</v>
@@ -10030,7 +10024,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -10046,16 +10040,16 @@
         <v>372</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D23" s="2">
-        <v>1.7749999999999999</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="E23" s="2">
-        <v>-4.9000000000000004</v>
+        <v>5.3</v>
       </c>
       <c r="F23" s="2">
-        <v>4.8</v>
+        <v>1.83</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>0</v>
@@ -10066,19 +10060,19 @@
         <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="D24" s="2">
-        <v>1.506</v>
+        <v>-3.9</v>
       </c>
       <c r="E24" s="2">
-        <v>-3.9</v>
+        <v>5.3</v>
       </c>
       <c r="F24" s="2">
-        <v>4.8</v>
+        <v>1.56</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>0</v>
@@ -10089,19 +10083,19 @@
         <v>3</v>
       </c>
       <c r="B25" s="1">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2">
-        <v>1.216</v>
+        <v>-2.1</v>
       </c>
       <c r="E25" s="2">
-        <v>-2.1</v>
+        <v>3.9</v>
       </c>
       <c r="F25" s="2">
-        <v>3.9</v>
+        <v>1.278</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>0</v>
@@ -10112,19 +10106,19 @@
         <v>4</v>
       </c>
       <c r="B26" s="1">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="D26" s="2">
-        <v>1.117</v>
+        <v>-2.1</v>
       </c>
       <c r="E26" s="2">
-        <v>-2.1</v>
+        <v>3.8</v>
       </c>
       <c r="F26" s="2">
-        <v>3.5</v>
+        <v>1.1759999999999999</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>0</v>
@@ -10135,19 +10129,19 @@
         <v>5</v>
       </c>
       <c r="B27" s="1">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D27" s="2">
-        <v>1.036</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="E27" s="2">
-        <v>-2.1</v>
+        <v>3.6</v>
       </c>
       <c r="F27" s="2">
-        <v>3.5</v>
+        <v>1.093</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>0</v>
@@ -10158,19 +10152,19 @@
         <v>6</v>
       </c>
       <c r="B28" s="1">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="D28" s="2">
-        <v>0.98399999999999999</v>
+        <v>-2.4</v>
       </c>
       <c r="E28" s="2">
-        <v>-2.2999999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="F28" s="2">
-        <v>3.1</v>
+        <v>1.042</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>0</v>
@@ -10181,19 +10175,19 @@
         <v>7</v>
       </c>
       <c r="B29" s="1">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="D29" s="2">
-        <v>0.88700000000000001</v>
+        <v>-2.4</v>
       </c>
       <c r="E29" s="2">
-        <v>-1.8</v>
+        <v>2.8</v>
       </c>
       <c r="F29" s="2">
-        <v>2.7</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>0</v>
@@ -10204,19 +10198,19 @@
         <v>8</v>
       </c>
       <c r="B30" s="1">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D30" s="2">
-        <v>0.74199999999999999</v>
+        <v>-2</v>
       </c>
       <c r="E30" s="2">
-        <v>-1.8</v>
+        <v>2.9</v>
       </c>
       <c r="F30" s="2">
-        <v>2.9</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>0</v>
@@ -10227,19 +10221,19 @@
         <v>9</v>
       </c>
       <c r="B31" s="1">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D31" s="2">
-        <v>0.60499999999999998</v>
+        <v>-2</v>
       </c>
       <c r="E31" s="2">
-        <v>-1.7</v>
+        <v>2.8</v>
       </c>
       <c r="F31" s="2">
-        <v>2.2000000000000002</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>0</v>
@@ -10250,19 +10244,19 @@
         <v>10</v>
       </c>
       <c r="B32" s="1">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D32" s="2">
-        <v>0.55200000000000005</v>
+        <v>-1.8</v>
       </c>
       <c r="E32" s="2">
-        <v>-1.7</v>
+        <v>2.7</v>
       </c>
       <c r="F32" s="2">
-        <v>2</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>0</v>
@@ -10273,19 +10267,19 @@
         <v>11</v>
       </c>
       <c r="B33" s="1">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2">
-        <v>0.434</v>
+        <v>-1</v>
       </c>
       <c r="E33" s="2">
-        <v>-0.9</v>
+        <v>2</v>
       </c>
       <c r="F33" s="2">
-        <v>1.7</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>0</v>
@@ -10296,19 +10290,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="1">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="C34" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="D34" s="2">
-        <v>0.318</v>
+        <v>-1.5</v>
       </c>
       <c r="E34" s="2">
-        <v>-1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F34" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>0</v>
@@ -10319,19 +10313,19 @@
         <v>13</v>
       </c>
       <c r="B35" s="1">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="C35" s="2">
         <v>-1E-3</v>
       </c>
       <c r="D35" s="2">
-        <v>0.218</v>
+        <v>-0.7</v>
       </c>
       <c r="E35" s="2">
-        <v>-0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F35" s="2">
-        <v>0.8</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>0</v>
@@ -10342,19 +10336,19 @@
         <v>14</v>
       </c>
       <c r="B36" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C36" s="2">
         <v>-1.7000000000000001E-2</v>
       </c>
       <c r="D36" s="2">
-        <v>0.313</v>
+        <v>-1</v>
       </c>
       <c r="E36" s="2">
-        <v>-1</v>
+        <v>1.6</v>
       </c>
       <c r="F36" s="2">
-        <v>1.6</v>
+        <v>0.31</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>0</v>
@@ -10371,13 +10365,13 @@
         <v>-4.5999999999999999E-2</v>
       </c>
       <c r="D37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="F37" s="2">
         <v>0.38100000000000001</v>
-      </c>
-      <c r="E37" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F37" s="2">
-        <v>1.6</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>0</v>
@@ -10394,13 +10388,13 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="D38" s="2">
+        <v>-0.6</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="F38" s="2">
         <v>0.36399999999999999</v>
-      </c>
-      <c r="E38" s="2">
-        <v>-0.6</v>
-      </c>
-      <c r="F38" s="2">
-        <v>1.6</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>0</v>
@@ -10417,13 +10411,13 @@
         <v>6.2E-2</v>
       </c>
       <c r="D39" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="F39" s="2">
         <v>0.36399999999999999</v>
-      </c>
-      <c r="E39" s="2">
-        <v>-0.4</v>
-      </c>
-      <c r="F39" s="2">
-        <v>1.6</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>0</v>
@@ -10477,7 +10471,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -10493,16 +10487,16 @@
         <v>372</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="D43" s="2">
-        <v>8.2759999999999998</v>
+        <v>-38.799999999999997</v>
       </c>
       <c r="E43" s="2">
-        <v>-32</v>
+        <v>23.5</v>
       </c>
       <c r="F43" s="2">
-        <v>21.4</v>
+        <v>15.125999999999999</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>0</v>
@@ -10513,19 +10507,19 @@
         <v>2</v>
       </c>
       <c r="B44" s="1">
-        <v>370</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>19</v>
+        <v>372</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1.18</v>
       </c>
       <c r="D44" s="2">
-        <v>8.0370000000000008</v>
+        <v>-38.799999999999997</v>
       </c>
       <c r="E44" s="2">
-        <v>-26.8</v>
+        <v>23.5</v>
       </c>
       <c r="F44" s="2">
-        <v>21</v>
+        <v>14.43</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>0</v>
@@ -10536,19 +10530,19 @@
         <v>3</v>
       </c>
       <c r="B45" s="1">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="D45" s="2">
-        <v>8.4060000000000006</v>
+        <v>-35.700000000000003</v>
       </c>
       <c r="E45" s="2">
-        <v>-26.7</v>
+        <v>23.5</v>
       </c>
       <c r="F45" s="2">
-        <v>21.4</v>
+        <v>10.24</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>0</v>
@@ -10559,19 +10553,19 @@
         <v>4</v>
       </c>
       <c r="B46" s="1">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C46" s="2">
-        <v>0.59599999999999997</v>
+        <v>0.126</v>
       </c>
       <c r="D46" s="2">
-        <v>7.4039999999999999</v>
+        <v>-35.700000000000003</v>
       </c>
       <c r="E46" s="2">
-        <v>-26.7</v>
+        <v>21.4</v>
       </c>
       <c r="F46" s="2">
-        <v>20.399999999999999</v>
+        <v>9.2550000000000008</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>0</v>
@@ -10582,19 +10576,19 @@
         <v>5</v>
       </c>
       <c r="B47" s="1">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="C47" s="2">
-        <v>0.20899999999999999</v>
+        <v>-0.32100000000000001</v>
       </c>
       <c r="D47" s="2">
-        <v>5.8289999999999997</v>
+        <v>-35.6</v>
       </c>
       <c r="E47" s="2">
-        <v>-25.3</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="F47" s="2">
-        <v>12.2</v>
+        <v>7.9489999999999998</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>0</v>
@@ -10605,19 +10599,19 @@
         <v>6</v>
       </c>
       <c r="B48" s="1">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="C48" s="2">
-        <v>0.128</v>
+        <v>-0.40600000000000003</v>
       </c>
       <c r="D48" s="2">
-        <v>5.3179999999999996</v>
+        <v>-32.4</v>
       </c>
       <c r="E48" s="2">
-        <v>-25.3</v>
+        <v>11.6</v>
       </c>
       <c r="F48" s="2">
-        <v>10.7</v>
+        <v>7.3220000000000001</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>0</v>
@@ -10628,19 +10622,19 @@
         <v>7</v>
       </c>
       <c r="B49" s="1">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="C49" s="2">
-        <v>0.315</v>
+        <v>-8.1000000000000003E-2</v>
       </c>
       <c r="D49" s="2">
-        <v>6.1660000000000004</v>
+        <v>-30.8</v>
       </c>
       <c r="E49" s="2">
-        <v>-24.4</v>
+        <v>12.9</v>
       </c>
       <c r="F49" s="2">
-        <v>10.7</v>
+        <v>7.6859999999999999</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>0</v>
@@ -10651,19 +10645,19 @@
         <v>8</v>
       </c>
       <c r="B50" s="1">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="C50" s="2">
-        <v>-0.184</v>
+        <v>-0.48699999999999999</v>
       </c>
       <c r="D50" s="2">
-        <v>5.2720000000000002</v>
+        <v>-32.4</v>
       </c>
       <c r="E50" s="2">
-        <v>-25.3</v>
+        <v>10.7</v>
       </c>
       <c r="F50" s="2">
-        <v>10</v>
+        <v>6.84</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>0</v>
@@ -10674,19 +10668,19 @@
         <v>9</v>
       </c>
       <c r="B51" s="1">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="C51" s="2">
-        <v>-0.109</v>
+        <v>-0.38800000000000001</v>
       </c>
       <c r="D51" s="2">
-        <v>4.5270000000000001</v>
+        <v>-26.6</v>
       </c>
       <c r="E51" s="2">
-        <v>-24.2</v>
+        <v>10.7</v>
       </c>
       <c r="F51" s="2">
-        <v>10</v>
+        <v>6.2130000000000001</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>0</v>
@@ -10697,19 +10691,19 @@
         <v>10</v>
       </c>
       <c r="B52" s="1">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="C52" s="2">
-        <v>-9.4E-2</v>
+        <v>-0.371</v>
       </c>
       <c r="D52" s="2">
-        <v>4.0359999999999996</v>
+        <v>-26.6</v>
       </c>
       <c r="E52" s="2">
-        <v>-19.7</v>
+        <v>9.9</v>
       </c>
       <c r="F52" s="2">
-        <v>9.9</v>
+        <v>5.6440000000000001</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>0</v>
@@ -10720,19 +10714,19 @@
         <v>11</v>
       </c>
       <c r="B53" s="1">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="C53" s="2">
-        <v>-0.13900000000000001</v>
+        <v>-0.442</v>
       </c>
       <c r="D53" s="2">
-        <v>3.496</v>
+        <v>-26.6</v>
       </c>
       <c r="E53" s="2">
-        <v>-19.7</v>
+        <v>7.8</v>
       </c>
       <c r="F53" s="2">
-        <v>7.8</v>
+        <v>5.3079999999999998</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>0</v>
@@ -10743,19 +10737,19 @@
         <v>12</v>
       </c>
       <c r="B54" s="1">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="D54" s="2">
-        <v>3.29</v>
+        <v>-25.3</v>
       </c>
       <c r="E54" s="2">
-        <v>-19.2</v>
+        <v>6.4</v>
       </c>
       <c r="F54" s="2">
-        <v>3.5</v>
+        <v>4.3289999999999997</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>0</v>
@@ -10766,19 +10760,19 @@
         <v>13</v>
       </c>
       <c r="B55" s="1">
-        <v>324</v>
+        <v>348</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D55" s="2">
-        <v>2.59</v>
+        <v>-13.1</v>
       </c>
       <c r="E55" s="2">
-        <v>-13.1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="2">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>0</v>
@@ -10789,19 +10783,19 @@
         <v>14</v>
       </c>
       <c r="B56" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C56" s="2">
-        <v>-1.0640000000000001</v>
+        <v>-1.0469999999999999</v>
       </c>
       <c r="D56" s="2">
-        <v>5.7850000000000001</v>
+        <v>-32.4</v>
       </c>
       <c r="E56" s="2">
-        <v>-32.4</v>
+        <v>6.4</v>
       </c>
       <c r="F56" s="2">
-        <v>6.4</v>
+        <v>5.7380000000000004</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>0</v>
@@ -10818,13 +10812,13 @@
         <v>-1.171</v>
       </c>
       <c r="D57" s="2">
+        <v>-32.4</v>
+      </c>
+      <c r="E57" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="F57" s="2">
         <v>6.1829999999999998</v>
-      </c>
-      <c r="E57" s="2">
-        <v>-32.4</v>
-      </c>
-      <c r="F57" s="2">
-        <v>6.4</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>0</v>
@@ -10841,13 +10835,13 @@
         <v>-1.04</v>
       </c>
       <c r="D58" s="2">
+        <v>-32.4</v>
+      </c>
+      <c r="E58" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="F58" s="2">
         <v>6.657</v>
-      </c>
-      <c r="E58" s="2">
-        <v>-32.4</v>
-      </c>
-      <c r="F58" s="2">
-        <v>6.4</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>0</v>
@@ -10864,13 +10858,13 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="D59" s="2">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="F59" s="2">
         <v>1.397</v>
-      </c>
-      <c r="E59" s="2">
-        <v>0</v>
-      </c>
-      <c r="F59" s="2">
-        <v>6.4</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>0</v>
@@ -10924,7 +10918,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -10940,7 +10934,7 @@
         <v>372</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D63" s="2">
         <v>1.333</v>
@@ -10963,7 +10957,7 @@
         <v>370</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D64" s="2">
         <v>1.165</v>
@@ -10986,7 +10980,7 @@
         <v>368</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D65" s="2">
         <v>0.997</v>
@@ -11009,7 +11003,7 @@
         <v>366</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D66" s="2">
         <v>0.877</v>
@@ -11032,7 +11026,7 @@
         <v>364</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D67" s="2">
         <v>0.81</v>
@@ -11055,7 +11049,7 @@
         <v>361</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D68" s="2">
         <v>0.78800000000000003</v>
@@ -11078,7 +11072,7 @@
         <v>358</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D69" s="2">
         <v>0.72799999999999998</v>
@@ -11101,7 +11095,7 @@
         <v>355</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D70" s="2">
         <v>0.71199999999999997</v>
@@ -11124,7 +11118,7 @@
         <v>352</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D71" s="2">
         <v>0.64100000000000001</v>
@@ -11147,7 +11141,7 @@
         <v>349</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D72" s="2">
         <v>0.57499999999999996</v>
@@ -11170,7 +11164,7 @@
         <v>346</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D73" s="2">
         <v>0.53600000000000003</v>
@@ -11371,7 +11365,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -11387,7 +11381,7 @@
         <v>372</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D83" s="2">
         <v>1.4590000000000001</v>
@@ -11410,7 +11404,7 @@
         <v>370</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D84" s="2">
         <v>1.3129999999999999</v>
@@ -11433,7 +11427,7 @@
         <v>368</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D85" s="2">
         <v>1.2490000000000001</v>
@@ -11456,7 +11450,7 @@
         <v>366</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D86" s="2">
         <v>1.157</v>
@@ -11479,7 +11473,7 @@
         <v>364</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D87" s="2">
         <v>0.96299999999999997</v>
@@ -11640,7 +11634,7 @@
         <v>343</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D94" s="2">
         <v>0.54600000000000004</v>
@@ -11663,7 +11657,7 @@
         <v>324</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D95" s="2">
         <v>0.314</v>
@@ -11818,7 +11812,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -11857,7 +11851,7 @@
         <v>260</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D104" s="2">
         <v>0.42899999999999999</v>
@@ -11880,7 +11874,7 @@
         <v>258</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D105" s="2">
         <v>0.44</v>
@@ -11903,7 +11897,7 @@
         <v>256</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D106" s="2">
         <v>0.35599999999999998</v>
@@ -11949,7 +11943,7 @@
         <v>251</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D108" s="2">
         <v>0.36099999999999999</v>
@@ -12150,7 +12144,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
@@ -12597,7 +12591,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
@@ -12613,7 +12607,7 @@
         <v>372</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D138" s="2">
         <v>1.976</v>
@@ -12636,7 +12630,7 @@
         <v>370</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D139" s="2">
         <v>1.7150000000000001</v>
@@ -12659,7 +12653,7 @@
         <v>368</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D140" s="2">
         <v>1.464</v>
@@ -12682,7 +12676,7 @@
         <v>366</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D141" s="2">
         <v>1.19</v>
@@ -12705,7 +12699,7 @@
         <v>364</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D142" s="2">
         <v>0.96</v>
@@ -12728,7 +12722,7 @@
         <v>361</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D143" s="2">
         <v>0.92</v>
@@ -12751,7 +12745,7 @@
         <v>358</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D144" s="2">
         <v>0.89600000000000002</v>
@@ -12774,7 +12768,7 @@
         <v>355</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D145" s="2">
         <v>0.88200000000000001</v>
@@ -12797,7 +12791,7 @@
         <v>352</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D146" s="2">
         <v>0.79200000000000004</v>
@@ -12820,7 +12814,7 @@
         <v>349</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D147" s="2">
         <v>0.71199999999999997</v>
@@ -12843,7 +12837,7 @@
         <v>346</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D148" s="2">
         <v>0.58499999999999996</v>
@@ -13044,7 +13038,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="8" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
@@ -13060,7 +13054,7 @@
         <v>332</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D158" s="5">
         <v>0.90200000000000002</v>

</xml_diff>